<commit_message>
Avances etiquetado de hoy
archivo excel nuevamente en lo que averiguo como irlo reemplazando. Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B78F188-4297-4415-A255-917734D7E5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A709EA-FB41-4D86-8ACA-EAFAF5E7F1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -476,7 +476,7 @@
   <dimension ref="D2:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,11 +551,21 @@
       <c r="D6" s="6">
         <v>45693</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="E6" s="5">
+        <v>370</v>
+      </c>
+      <c r="F6" s="5">
+        <v>355</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="4:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D7" s="5"/>

</xml_diff>

<commit_message>
Avances Etiquetado Lunes 05 Mayo
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A709EA-FB41-4D86-8ACA-EAFAF5E7F1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4B10EA-21E5-494E-AABD-42473DF93E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Fecha</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>Etiquetado Covenant Drone</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se subieron 300 imagenes a dataset </t>
   </si>
 </sst>
 </file>
@@ -473,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:I11"/>
+  <dimension ref="D2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,10 +495,10 @@
     <col min="6" max="6" width="31.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="49.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="41.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -499,7 +508,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="4:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -507,7 +516,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="4:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D4" s="4" t="s">
         <v>0</v>
       </c>
@@ -526,8 +535,11 @@
       <c r="I4" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="4:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
@@ -546,8 +558,11 @@
       <c r="I5" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="4:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D6" s="6">
         <v>45693</v>
       </c>
@@ -566,46 +581,68 @@
       <c r="I6" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="4:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="4:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J6" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D7" s="6">
+        <v>45782</v>
+      </c>
+      <c r="E7" s="5">
+        <v>585</v>
+      </c>
+      <c r="F7" s="5">
+        <v>202</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>300</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="4:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="4:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Avances etiquetado Martes 05/06/2025
saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4B10EA-21E5-494E-AABD-42473DF93E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC69B550-CD83-4293-9727-9DAA30813FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Fecha</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t xml:space="preserve">Se subieron 300 imagenes a dataset </t>
+  </si>
+  <si>
+    <t>hoy no pude etiquetar (rafael), mañana me aventare el doble, saludos</t>
   </si>
 </sst>
 </file>
@@ -484,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,7 +498,8 @@
     <col min="6" max="6" width="31.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="49.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="64" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -609,13 +613,27 @@
       </c>
     </row>
     <row r="8" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="D8" s="6">
+        <v>45813</v>
+      </c>
+      <c r="E8" s="5">
+        <v>562</v>
+      </c>
+      <c r="F8" s="5">
+        <v>226</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>300</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D9" s="5"/>

</xml_diff>

<commit_message>
Avances etiquetado Miercoles 05/07/2025
saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC69B550-CD83-4293-9727-9DAA30813FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED8C0DB-F0F7-4626-B408-9C7C188A70B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Fecha</t>
   </si>
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,13 +636,27 @@
       </c>
     </row>
     <row r="9" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="D9" s="6">
+        <v>45843</v>
+      </c>
+      <c r="E9" s="5">
+        <v>419</v>
+      </c>
+      <c r="F9" s="5">
+        <v>367</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>300</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D10" s="5"/>

</xml_diff>

<commit_message>
Avances etiquetado Jueves 5/8/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED8C0DB-F0F7-4626-B408-9C7C188A70B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F670D425-9861-4A4C-9F36-67C9329E1561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Fecha</t>
   </si>
@@ -488,7 +488,7 @@
   <dimension ref="D2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,13 +659,27 @@
       </c>
     </row>
     <row r="10" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="D10" s="6">
+        <v>45874</v>
+      </c>
+      <c r="E10" s="5">
+        <v>364</v>
+      </c>
+      <c r="F10" s="5">
+        <v>419</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>300</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D11" s="1"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow Viernes 5/9/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F670D425-9861-4A4C-9F36-67C9329E1561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6786234C-0BA5-418F-BC78-1C982C786038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Fecha</t>
   </si>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Se subieron 300 imagenes a dataset </t>
   </si>
   <si>
-    <t>hoy no pude etiquetar (rafael), mañana me aventare el doble, saludos</t>
+    <t xml:space="preserve">Este fin se vienen las fotos que no pude adelantar en la semana (rafael) </t>
   </si>
 </sst>
 </file>
@@ -143,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -151,6 +151,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,7 +489,7 @@
   <dimension ref="D2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,7 +633,7 @@
         <v>300</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -682,13 +683,27 @@
       </c>
     </row>
     <row r="11" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="D11" s="7">
+        <v>45905</v>
+      </c>
+      <c r="E11" s="1">
+        <v>359</v>
+      </c>
+      <c r="F11" s="1">
+        <v>424</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>300</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow Jueves 5/15/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1F3176-DA66-4D27-9665-8B697110ED93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFC82D1-0678-4888-A282-72B2AB4C2358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>Fecha</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>no he podido etiquetar una disculpa (rafael)</t>
+  </si>
+  <si>
+    <t>15/5/2025</t>
+  </si>
+  <si>
+    <t>16/5/2025</t>
   </si>
 </sst>
 </file>
@@ -254,21 +260,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -280,8 +281,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,6 +551,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -563,13 +589,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -619,8 +638,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J15" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J15" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J19" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -951,21 +970,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J15"/>
+  <dimension ref="D2:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="8" max="8" width="52.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="62.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -987,25 +1007,25 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D4" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1028,12 +1048,12 @@
       <c r="I5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="16" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="4">
@@ -1051,12 +1071,12 @@
       <c r="I6" s="4">
         <v>0</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D7" s="7">
+      <c r="D7" s="17">
         <v>45693</v>
       </c>
       <c r="E7" s="4">
@@ -1074,12 +1094,12 @@
       <c r="I7" s="4">
         <v>0</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D8" s="7">
+      <c r="D8" s="17">
         <v>45782</v>
       </c>
       <c r="E8" s="4">
@@ -1097,12 +1117,12 @@
       <c r="I8" s="4">
         <v>300</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D9" s="7">
+      <c r="D9" s="17">
         <v>45813</v>
       </c>
       <c r="E9" s="4">
@@ -1120,12 +1140,12 @@
       <c r="I9" s="4">
         <v>300</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D10" s="7">
+      <c r="D10" s="17">
         <v>45843</v>
       </c>
       <c r="E10" s="4">
@@ -1143,12 +1163,12 @@
       <c r="I10" s="4">
         <v>300</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D11" s="7">
+      <c r="D11" s="17">
         <v>45874</v>
       </c>
       <c r="E11" s="4">
@@ -1166,101 +1186,180 @@
       <c r="I11" s="4">
         <v>300</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D12" s="10">
+      <c r="D12" s="18">
         <v>45905</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="8">
         <v>359</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="8">
         <v>424</v>
       </c>
-      <c r="G12" s="11">
-        <v>0</v>
-      </c>
-      <c r="H12" s="11">
-        <v>0</v>
-      </c>
-      <c r="I12" s="11">
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0</v>
+      </c>
+      <c r="I12" s="8">
         <v>300</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="21" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D13" s="13">
+      <c r="D13" s="14">
         <v>45996</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="9">
         <v>344</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="9">
         <v>315</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="9">
         <v>37</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="9">
         <v>80</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="9">
         <v>300</v>
       </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="22" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="9">
         <v>344</v>
       </c>
-      <c r="F14" s="14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="14">
+      <c r="F14" s="9">
+        <v>0</v>
+      </c>
+      <c r="G14" s="9">
         <v>74</v>
       </c>
-      <c r="H14" s="14">
-        <v>0</v>
-      </c>
-      <c r="I14" s="14">
+      <c r="H14" s="9">
+        <v>0</v>
+      </c>
+      <c r="I14" s="9">
         <v>650</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="J14" s="22" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="15">
         <v>306</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="15">
         <v>36</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="15">
         <v>74</v>
       </c>
-      <c r="H15" s="20">
-        <v>0</v>
-      </c>
-      <c r="I15" s="20">
+      <c r="H15" s="15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="15">
         <v>650</v>
       </c>
-      <c r="J15" s="21" t="s">
+      <c r="J15" s="22" t="s">
         <v>14</v>
       </c>
+    </row>
+    <row r="16" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="9">
+        <v>281</v>
+      </c>
+      <c r="F16" s="9">
+        <v>75</v>
+      </c>
+      <c r="G16" s="9">
+        <v>60</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0</v>
+      </c>
+      <c r="I16" s="9">
+        <v>650</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D17" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D18" s="17"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D19" s="14"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="10"/>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D21" s="19"/>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D24" s="19"/>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D25" s="19"/>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D26" s="19"/>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D27" s="19"/>
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D28" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Avances Etiquetado Viernes 5/16/2025
Saludos buen fin de semana
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFC82D1-0678-4888-A282-72B2AB4C2358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D539FAAF-D6CD-4E54-AC12-712983097287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Fecha</t>
   </si>
@@ -551,13 +551,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -589,6 +582,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -638,7 +638,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="D4:J19" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
@@ -973,7 +973,7 @@
   <dimension ref="D2:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1309,12 +1309,24 @@
       <c r="D17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="7"/>
+      <c r="E17" s="4">
+        <v>276</v>
+      </c>
+      <c r="F17" s="4">
+        <v>80</v>
+      </c>
+      <c r="G17" s="4">
+        <v>60</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>650</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="18" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D18" s="17"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 5/19/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D539FAAF-D6CD-4E54-AC12-712983097287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A737F652-16F1-49A6-BEF7-B495096E18A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>Fecha</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>16/5/2025</t>
+  </si>
+  <si>
+    <t>19/5/2025</t>
   </si>
 </sst>
 </file>
@@ -973,7 +976,7 @@
   <dimension ref="D2:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1329,13 +1332,27 @@
       </c>
     </row>
     <row r="18" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D18" s="17"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="7"/>
+      <c r="D18" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="4">
+        <v>135</v>
+      </c>
+      <c r="F18" s="4">
+        <v>218</v>
+      </c>
+      <c r="G18" s="4">
+        <v>60</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>650</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="19" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D19" s="14"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 5/20/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A737F652-16F1-49A6-BEF7-B495096E18A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E14F46-C2FD-45E6-AA6D-CAD012463A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>Fecha</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>19/5/2025</t>
+  </si>
+  <si>
+    <t>20/5/2025</t>
+  </si>
+  <si>
+    <t>no he podido etiquetar por examenes finales una disculpa (rafael)</t>
   </si>
 </sst>
 </file>
@@ -641,8 +647,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J19" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J20" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J20" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -976,7 +982,7 @@
   <dimension ref="D2:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1355,16 +1361,36 @@
       </c>
     </row>
     <row r="19" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D19" s="14"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="10"/>
-    </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D20" s="19"/>
+      <c r="D19" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="9">
+        <v>135</v>
+      </c>
+      <c r="F19" s="9">
+        <v>218</v>
+      </c>
+      <c r="G19" s="9">
+        <v>60</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0</v>
+      </c>
+      <c r="I19" s="9">
+        <v>650</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D20" s="14"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D21" s="19"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 5/21/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E14F46-C2FD-45E6-AA6D-CAD012463A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF1780B-485D-41E2-9294-13BC9FA1CCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Fecha</t>
   </si>
@@ -96,13 +96,25 @@
   </si>
   <si>
     <t>no he podido etiquetar por examenes finales una disculpa (rafael)</t>
+  </si>
+  <si>
+    <t>21/5/2025</t>
+  </si>
+  <si>
+    <t>a partir de mañana me regularizo con el etiquetado (rafael)</t>
+  </si>
+  <si>
+    <t>22/5/2025</t>
+  </si>
+  <si>
+    <t>23/5/2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +133,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -647,8 +665,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J20" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J20" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J24" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J24" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -982,7 +1000,7 @@
   <dimension ref="D2:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1384,25 +1402,67 @@
       </c>
     </row>
     <row r="20" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D20" s="14"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="10"/>
-    </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D21" s="19"/>
-    </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D22" s="19"/>
-    </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D23" s="19"/>
-    </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D24" s="19"/>
+      <c r="D20" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="9">
+        <v>178</v>
+      </c>
+      <c r="F20" s="9">
+        <v>328</v>
+      </c>
+      <c r="G20" s="9">
+        <v>60</v>
+      </c>
+      <c r="H20" s="9">
+        <v>0</v>
+      </c>
+      <c r="I20" s="9">
+        <v>650</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D21" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D22" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D23" s="17"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D24" s="14"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="10"/>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D25" s="19"/>
@@ -1417,6 +1477,7 @@
       <c r="D28" s="19"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow Jueves 5/22/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF1780B-485D-41E2-9294-13BC9FA1CCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C285FFE3-AC7E-4EE1-88F5-E426D65DB32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Fecha</t>
   </si>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1428,12 +1428,24 @@
       <c r="D21" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="7"/>
+      <c r="E21" s="4">
+        <v>178</v>
+      </c>
+      <c r="F21" s="4">
+        <v>339</v>
+      </c>
+      <c r="G21" s="4">
+        <v>49</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>650</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="22" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D22" s="17" t="s">

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow Viernes 5/23/2025
Saludos, buen fin de semana
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C285FFE3-AC7E-4EE1-88F5-E426D65DB32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06390ABA-44B4-46A4-9D65-5D8C2743E5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Fecha</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>23/5/2025</t>
+  </si>
+  <si>
+    <t>Seguire trabajando en fin de semana (rafael)</t>
   </si>
 </sst>
 </file>
@@ -999,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1451,12 +1454,24 @@
       <c r="D22" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="7"/>
+      <c r="E22" s="4">
+        <v>175</v>
+      </c>
+      <c r="F22" s="4">
+        <v>357</v>
+      </c>
+      <c r="G22" s="4">
+        <v>34</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>650</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="23" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D23" s="17"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow Lunes 5/26/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06390ABA-44B4-46A4-9D65-5D8C2743E5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC164B6-D1CE-4D26-8C53-9F51040D5BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Fecha</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Seguire trabajando en fin de semana (rafael)</t>
+  </si>
+  <si>
+    <t>26/5/2025</t>
   </si>
 </sst>
 </file>
@@ -1002,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1474,13 +1477,27 @@
       </c>
     </row>
     <row r="23" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D23" s="17"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="7"/>
+      <c r="D23" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="4">
+        <v>125</v>
+      </c>
+      <c r="F23" s="4">
+        <v>426</v>
+      </c>
+      <c r="G23" s="4">
+        <v>15</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4">
+        <v>650</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="24" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D24" s="14"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow Miercoles 5/28/2025
Saludos, ayer github no me dejo subir el avance del martes, una disculpa
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC164B6-D1CE-4D26-8C53-9F51040D5BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACB75CF-0895-4D92-96D7-47220064B930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>Fecha</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>26/5/2025</t>
+  </si>
+  <si>
+    <t>27/5/2025</t>
+  </si>
+  <si>
+    <t>28/5/2025</t>
   </si>
 </sst>
 </file>
@@ -671,8 +677,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J24" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J24" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J26" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1005,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1500,19 +1506,59 @@
       </c>
     </row>
     <row r="24" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D24" s="14"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="10"/>
-    </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D25" s="19"/>
-    </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D26" s="19"/>
+      <c r="D24" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="9">
+        <v>125</v>
+      </c>
+      <c r="F24" s="9">
+        <v>441</v>
+      </c>
+      <c r="G24" s="9">
+        <v>0</v>
+      </c>
+      <c r="H24" s="9">
+        <v>0</v>
+      </c>
+      <c r="I24" s="9">
+        <v>650</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D25" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="4">
+        <v>110</v>
+      </c>
+      <c r="F25" s="4">
+        <v>456</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4">
+        <v>650</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D26" s="14"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="10"/>
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D27" s="19"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 5/29/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACB75CF-0895-4D92-96D7-47220064B930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF0CE55-5828-4800-B792-1F159981C57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>Fecha</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>28/5/2025</t>
+  </si>
+  <si>
+    <t>29/5/2025</t>
   </si>
 </sst>
 </file>
@@ -1011,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1552,13 +1555,27 @@
       </c>
     </row>
     <row r="26" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D26" s="14"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="10"/>
+      <c r="D26" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="9">
+        <v>90</v>
+      </c>
+      <c r="F26" s="9">
+        <v>476</v>
+      </c>
+      <c r="G26" s="9">
+        <v>0</v>
+      </c>
+      <c r="H26" s="9">
+        <v>0</v>
+      </c>
+      <c r="I26" s="9">
+        <v>650</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D27" s="19"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 5/30/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF0CE55-5828-4800-B792-1F159981C57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29991E5A-149D-453F-92C0-2B8B8605B452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>Fecha</t>
   </si>
@@ -59,9 +59,6 @@
     <t>29/04/2025-01/05/2025</t>
   </si>
   <si>
-    <t>Etiquetado Covenant Drone</t>
-  </si>
-  <si>
     <t>Notas</t>
   </si>
   <si>
@@ -123,6 +120,12 @@
   </si>
   <si>
     <t>29/5/2025</t>
+  </si>
+  <si>
+    <t>Etiquetado Roboflow Covenant Drone</t>
+  </si>
+  <si>
+    <t>30/5/2025</t>
   </si>
 </sst>
 </file>
@@ -302,10 +305,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -332,9 +334,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -343,6 +342,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,8 +684,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J26" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J45" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J45" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1012,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J28"/>
+  <dimension ref="D2:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,8 +1038,8 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
+      <c r="G2" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1049,539 +1053,718 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="D4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3">
+        <v>450</v>
+      </c>
+      <c r="F6" s="3">
+        <v>275</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="6" t="s">
+    <row r="7" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D7" s="16">
+        <v>45693</v>
+      </c>
+      <c r="E7" s="3">
+        <v>370</v>
+      </c>
+      <c r="F7" s="3">
+        <v>355</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D6" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="4">
-        <v>450</v>
-      </c>
-      <c r="F6" s="4">
-        <v>275</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="20" t="s">
+    <row r="8" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D8" s="16">
+        <v>45782</v>
+      </c>
+      <c r="E8" s="3">
+        <v>585</v>
+      </c>
+      <c r="F8" s="3">
+        <v>202</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>300</v>
+      </c>
+      <c r="J8" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D7" s="17">
-        <v>45693</v>
-      </c>
-      <c r="E7" s="4">
-        <v>370</v>
-      </c>
-      <c r="F7" s="4">
-        <v>355</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D8" s="17">
-        <v>45782</v>
-      </c>
-      <c r="E8" s="4">
-        <v>585</v>
-      </c>
-      <c r="F8" s="4">
-        <v>202</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
+    <row r="9" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D9" s="16">
+        <v>45813</v>
+      </c>
+      <c r="E9" s="3">
+        <v>562</v>
+      </c>
+      <c r="F9" s="3">
+        <v>226</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
         <v>300</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J9" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D10" s="16">
+        <v>45843</v>
+      </c>
+      <c r="E10" s="3">
+        <v>419</v>
+      </c>
+      <c r="F10" s="3">
+        <v>367</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>300</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D11" s="16">
+        <v>45874</v>
+      </c>
+      <c r="E11" s="3">
+        <v>364</v>
+      </c>
+      <c r="F11" s="3">
+        <v>419</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>300</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D12" s="17">
+        <v>45905</v>
+      </c>
+      <c r="E12" s="7">
+        <v>359</v>
+      </c>
+      <c r="F12" s="7">
+        <v>424</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7">
+        <v>300</v>
+      </c>
+      <c r="J12" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D9" s="17">
-        <v>45813</v>
-      </c>
-      <c r="E9" s="4">
-        <v>562</v>
-      </c>
-      <c r="F9" s="4">
-        <v>226</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
+    <row r="13" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D13" s="13">
+        <v>45996</v>
+      </c>
+      <c r="E13" s="8">
+        <v>344</v>
+      </c>
+      <c r="F13" s="8">
+        <v>315</v>
+      </c>
+      <c r="G13" s="8">
+        <v>37</v>
+      </c>
+      <c r="H13" s="8">
+        <v>80</v>
+      </c>
+      <c r="I13" s="8">
         <v>300</v>
       </c>
-      <c r="J9" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D10" s="17">
-        <v>45843</v>
-      </c>
-      <c r="E10" s="4">
-        <v>419</v>
-      </c>
-      <c r="F10" s="4">
-        <v>367</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
-        <v>300</v>
-      </c>
-      <c r="J10" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D11" s="17">
-        <v>45874</v>
-      </c>
-      <c r="E11" s="4">
-        <v>364</v>
-      </c>
-      <c r="F11" s="4">
-        <v>419</v>
-      </c>
-      <c r="G11" s="4">
-        <v>0</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4">
-        <v>300</v>
-      </c>
-      <c r="J11" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D12" s="18">
-        <v>45905</v>
-      </c>
-      <c r="E12" s="8">
-        <v>359</v>
-      </c>
-      <c r="F12" s="8">
-        <v>424</v>
-      </c>
-      <c r="G12" s="8">
-        <v>0</v>
-      </c>
-      <c r="H12" s="8">
-        <v>0</v>
-      </c>
-      <c r="I12" s="8">
-        <v>300</v>
-      </c>
-      <c r="J12" s="21" t="s">
+      <c r="J13" s="20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D14" s="13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D13" s="14">
-        <v>45996</v>
-      </c>
-      <c r="E13" s="9">
+      <c r="E14" s="8">
         <v>344</v>
       </c>
-      <c r="F13" s="9">
-        <v>315</v>
-      </c>
-      <c r="G13" s="9">
-        <v>37</v>
-      </c>
-      <c r="H13" s="9">
+      <c r="F14" s="8">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>74</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0</v>
+      </c>
+      <c r="I14" s="8">
+        <v>650</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="14">
+        <v>306</v>
+      </c>
+      <c r="F15" s="14">
+        <v>36</v>
+      </c>
+      <c r="G15" s="14">
+        <v>74</v>
+      </c>
+      <c r="H15" s="14">
+        <v>0</v>
+      </c>
+      <c r="I15" s="14">
+        <v>650</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="8">
+        <v>281</v>
+      </c>
+      <c r="F16" s="8">
+        <v>75</v>
+      </c>
+      <c r="G16" s="8">
+        <v>60</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0</v>
+      </c>
+      <c r="I16" s="8">
+        <v>650</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="3">
+        <v>276</v>
+      </c>
+      <c r="F17" s="3">
         <v>80</v>
       </c>
-      <c r="I13" s="9">
-        <v>300</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D14" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="9">
-        <v>344</v>
-      </c>
-      <c r="F14" s="9">
-        <v>0</v>
-      </c>
-      <c r="G14" s="9">
-        <v>74</v>
-      </c>
-      <c r="H14" s="9">
-        <v>0</v>
-      </c>
-      <c r="I14" s="9">
+      <c r="G17" s="3">
+        <v>60</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
         <v>650</v>
       </c>
-      <c r="J14" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D15" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="15">
-        <v>306</v>
-      </c>
-      <c r="F15" s="15">
-        <v>36</v>
-      </c>
-      <c r="G15" s="15">
-        <v>74</v>
-      </c>
-      <c r="H15" s="15">
-        <v>0</v>
-      </c>
-      <c r="I15" s="15">
+      <c r="J17" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D18" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="3">
+        <v>135</v>
+      </c>
+      <c r="F18" s="3">
+        <v>218</v>
+      </c>
+      <c r="G18" s="3">
+        <v>60</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
         <v>650</v>
       </c>
-      <c r="J15" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D16" s="14" t="s">
+      <c r="J18" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D19" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="8">
+        <v>135</v>
+      </c>
+      <c r="F19" s="8">
+        <v>218</v>
+      </c>
+      <c r="G19" s="8">
+        <v>60</v>
+      </c>
+      <c r="H19" s="8">
+        <v>0</v>
+      </c>
+      <c r="I19" s="8">
+        <v>650</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D20" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="8">
+        <v>178</v>
+      </c>
+      <c r="F20" s="8">
+        <v>328</v>
+      </c>
+      <c r="G20" s="8">
+        <v>60</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0</v>
+      </c>
+      <c r="I20" s="8">
+        <v>650</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="3">
+        <v>178</v>
+      </c>
+      <c r="F21" s="3">
+        <v>339</v>
+      </c>
+      <c r="G21" s="3">
+        <v>49</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <v>650</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D22" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="3">
+        <v>175</v>
+      </c>
+      <c r="F22" s="3">
+        <v>357</v>
+      </c>
+      <c r="G22" s="3">
+        <v>34</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>650</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D23" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="3">
+        <v>125</v>
+      </c>
+      <c r="F23" s="3">
+        <v>426</v>
+      </c>
+      <c r="G23" s="3">
         <v>15</v>
       </c>
-      <c r="E16" s="9">
-        <v>281</v>
-      </c>
-      <c r="F16" s="9">
-        <v>75</v>
-      </c>
-      <c r="G16" s="9">
-        <v>60</v>
-      </c>
-      <c r="H16" s="9">
-        <v>0</v>
-      </c>
-      <c r="I16" s="9">
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
         <v>650</v>
       </c>
-      <c r="J16" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D17" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="4">
-        <v>276</v>
-      </c>
-      <c r="F17" s="4">
-        <v>80</v>
-      </c>
-      <c r="G17" s="4">
-        <v>60</v>
-      </c>
-      <c r="H17" s="4">
-        <v>0</v>
-      </c>
-      <c r="I17" s="4">
+      <c r="J23" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D24" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="8">
+        <v>125</v>
+      </c>
+      <c r="F24" s="8">
+        <v>441</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0</v>
+      </c>
+      <c r="H24" s="8">
+        <v>0</v>
+      </c>
+      <c r="I24" s="8">
         <v>650</v>
       </c>
-      <c r="J17" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D18" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="4">
-        <v>135</v>
-      </c>
-      <c r="F18" s="4">
-        <v>218</v>
-      </c>
-      <c r="G18" s="4">
-        <v>60</v>
-      </c>
-      <c r="H18" s="4">
-        <v>0</v>
-      </c>
-      <c r="I18" s="4">
+      <c r="J24" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D25" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="3">
+        <v>110</v>
+      </c>
+      <c r="F25" s="3">
+        <v>456</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
         <v>650</v>
       </c>
-      <c r="J18" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D19" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="9">
-        <v>135</v>
-      </c>
-      <c r="F19" s="9">
-        <v>218</v>
-      </c>
-      <c r="G19" s="9">
-        <v>60</v>
-      </c>
-      <c r="H19" s="9">
-        <v>0</v>
-      </c>
-      <c r="I19" s="9">
+      <c r="J25" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D26" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="8">
+        <v>90</v>
+      </c>
+      <c r="F26" s="8">
+        <v>476</v>
+      </c>
+      <c r="G26" s="8">
+        <v>0</v>
+      </c>
+      <c r="H26" s="8">
+        <v>0</v>
+      </c>
+      <c r="I26" s="8">
         <v>650</v>
       </c>
-      <c r="J19" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D20" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="9">
-        <v>178</v>
-      </c>
-      <c r="F20" s="9">
-        <v>328</v>
-      </c>
-      <c r="G20" s="9">
-        <v>60</v>
-      </c>
-      <c r="H20" s="9">
-        <v>0</v>
-      </c>
-      <c r="I20" s="9">
+      <c r="J26" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D27" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="3">
+        <v>70</v>
+      </c>
+      <c r="F27" s="3">
+        <v>496</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
         <v>650</v>
       </c>
-      <c r="J20" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D21" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="4">
-        <v>178</v>
-      </c>
-      <c r="F21" s="4">
-        <v>339</v>
-      </c>
-      <c r="G21" s="4">
-        <v>49</v>
-      </c>
-      <c r="H21" s="4">
-        <v>0</v>
-      </c>
-      <c r="I21" s="4">
-        <v>650</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D22" s="17" t="s">
+      <c r="J27" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="4">
-        <v>175</v>
-      </c>
-      <c r="F22" s="4">
-        <v>357</v>
-      </c>
-      <c r="G22" s="4">
-        <v>34</v>
-      </c>
-      <c r="H22" s="4">
-        <v>0</v>
-      </c>
-      <c r="I22" s="4">
-        <v>650</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D23" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="4">
-        <v>125</v>
-      </c>
-      <c r="F23" s="4">
-        <v>426</v>
-      </c>
-      <c r="G23" s="4">
-        <v>15</v>
-      </c>
-      <c r="H23" s="4">
-        <v>0</v>
-      </c>
-      <c r="I23" s="4">
-        <v>650</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D24" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="9">
-        <v>125</v>
-      </c>
-      <c r="F24" s="9">
-        <v>441</v>
-      </c>
-      <c r="G24" s="9">
-        <v>0</v>
-      </c>
-      <c r="H24" s="9">
-        <v>0</v>
-      </c>
-      <c r="I24" s="9">
-        <v>650</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D25" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="4">
-        <v>110</v>
-      </c>
-      <c r="F25" s="4">
-        <v>456</v>
-      </c>
-      <c r="G25" s="4">
-        <v>0</v>
-      </c>
-      <c r="H25" s="4">
-        <v>0</v>
-      </c>
-      <c r="I25" s="4">
-        <v>650</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D26" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="9">
-        <v>90</v>
-      </c>
-      <c r="F26" s="9">
-        <v>476</v>
-      </c>
-      <c r="G26" s="9">
-        <v>0</v>
-      </c>
-      <c r="H26" s="9">
-        <v>0</v>
-      </c>
-      <c r="I26" s="9">
-        <v>650</v>
-      </c>
-      <c r="J26" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D27" s="19"/>
-    </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D28" s="19"/>
+    </row>
+    <row r="28" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D28" s="16"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="6"/>
+    </row>
+    <row r="29" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D29" s="21"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D30" s="21"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D31" s="21"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="6"/>
+    </row>
+    <row r="32" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D32" s="22"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D33" s="21"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D34" s="21"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D35" s="21"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D36" s="21"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="6"/>
+    </row>
+    <row r="37" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D37" s="22"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="9"/>
+    </row>
+    <row r="38" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D38" s="21"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D39" s="21"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="6"/>
+    </row>
+    <row r="40" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D40" s="21"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="6"/>
+    </row>
+    <row r="41" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D41" s="21"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="6"/>
+    </row>
+    <row r="42" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D42" s="21"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="6"/>
+    </row>
+    <row r="43" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D43" s="21"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="6"/>
+    </row>
+    <row r="44" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D44" s="22"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="9"/>
+    </row>
+    <row r="45" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D45" s="22"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 6/3/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29991E5A-149D-453F-92C0-2B8B8605B452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A485C87-2B75-4309-9730-50333F47891E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>Fecha</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>30/5/2025</t>
+  </si>
+  <si>
+    <t>2-3/6/2025</t>
   </si>
 </sst>
 </file>
@@ -1018,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1605,16 +1608,32 @@
       </c>
     </row>
     <row r="28" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D28" s="16"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="6"/>
+      <c r="D28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="3">
+        <v>127</v>
+      </c>
+      <c r="F28" s="3">
+        <v>234</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="29" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D29" s="21"/>
+      <c r="D29" s="21">
+        <v>45753</v>
+      </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -1623,7 +1642,9 @@
       <c r="J29" s="6"/>
     </row>
     <row r="30" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D30" s="21"/>
+      <c r="D30" s="21">
+        <v>45783</v>
+      </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 6/4/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A485C87-2B75-4309-9730-50333F47891E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74156ACF-43EA-447C-A571-0726605FB923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>Fecha</t>
   </si>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1634,12 +1634,24 @@
       <c r="D29" s="21">
         <v>45753</v>
       </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="6"/>
+      <c r="E29" s="3">
+        <v>127</v>
+      </c>
+      <c r="F29" s="3">
+        <v>234</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="30" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D30" s="21">

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 6/5/2025
saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74156ACF-43EA-447C-A571-0726605FB923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99682FAE-8BE6-41B0-A8FF-1C80231681AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>Fecha</t>
   </si>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1657,12 +1657,24 @@
       <c r="D30" s="21">
         <v>45783</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="6"/>
+      <c r="E30" s="3">
+        <v>127</v>
+      </c>
+      <c r="F30" s="3">
+        <v>234</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="31" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D31" s="21"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 6/6/2025
Saludos, buen fin de semana
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99682FAE-8BE6-41B0-A8FF-1C80231681AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4C5F72-FF99-4C86-B05B-4D62663B7757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>Fecha</t>
   </si>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1677,13 +1677,27 @@
       </c>
     </row>
     <row r="31" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D31" s="21"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="6"/>
+      <c r="D31" s="21">
+        <v>45814</v>
+      </c>
+      <c r="E31" s="3">
+        <v>100</v>
+      </c>
+      <c r="F31" s="3">
+        <v>261</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="32" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D32" s="22"/>

</xml_diff>

<commit_message>
Avances etiquetado roboflow 6/9/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4C5F72-FF99-4C86-B05B-4D62663B7757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D979F649-EE36-4321-8BC4-80CF8AE77D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>Fecha</t>
   </si>
@@ -1022,7 +1022,7 @@
   <dimension ref="D2:J45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1700,13 +1700,27 @@
       </c>
     </row>
     <row r="32" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D32" s="22"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="9"/>
+      <c r="D32" s="22">
+        <v>45906</v>
+      </c>
+      <c r="E32" s="8">
+        <v>95</v>
+      </c>
+      <c r="F32" s="8">
+        <v>423</v>
+      </c>
+      <c r="G32" s="8">
+        <v>0</v>
+      </c>
+      <c r="H32" s="8">
+        <v>0</v>
+      </c>
+      <c r="I32" s="8">
+        <v>1012</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="33" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D33" s="21"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 6/10/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D979F649-EE36-4321-8BC4-80CF8AE77D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9026B9E5-0915-4D5C-88B9-3C74941FF1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
   <si>
     <t>Fecha</t>
   </si>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1723,13 +1723,27 @@
       </c>
     </row>
     <row r="33" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D33" s="21"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="6"/>
+      <c r="D33" s="21">
+        <v>45936</v>
+      </c>
+      <c r="E33" s="3">
+        <v>75</v>
+      </c>
+      <c r="F33" s="3">
+        <v>443</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="34" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D34" s="21"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 6/11/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9026B9E5-0915-4D5C-88B9-3C74941FF1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA76DC3-FA2A-4643-B389-089F940C728B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>Fecha</t>
   </si>
@@ -1022,7 +1022,7 @@
   <dimension ref="D2:J45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1746,13 +1746,27 @@
       </c>
     </row>
     <row r="34" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D34" s="21"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="6"/>
+      <c r="D34" s="21">
+        <v>45967</v>
+      </c>
+      <c r="E34" s="3">
+        <v>75</v>
+      </c>
+      <c r="F34" s="3">
+        <v>443</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="35" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D35" s="21"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 6/12/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA76DC3-FA2A-4643-B389-089F940C728B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6340C0D3-C8FB-475D-9143-A95C008723E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>Fecha</t>
   </si>
@@ -1022,7 +1022,7 @@
   <dimension ref="D2:J45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1769,13 +1769,27 @@
       </c>
     </row>
     <row r="35" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D35" s="21"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="6"/>
+      <c r="D35" s="21">
+        <v>45997</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>518</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="36" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D36" s="21"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 6/13/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6340C0D3-C8FB-475D-9143-A95C008723E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC61948B-20BF-4EB6-A314-D1A5138CF6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>Fecha</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>2-3/6/2025</t>
+  </si>
+  <si>
+    <t>13/6/2025</t>
   </si>
 </sst>
 </file>
@@ -308,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -350,6 +353,9 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1021,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1792,13 +1798,27 @@
       </c>
     </row>
     <row r="36" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D36" s="21"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="6"/>
+      <c r="D36" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="24">
+        <v>0</v>
+      </c>
+      <c r="F36" s="24">
+        <v>518</v>
+      </c>
+      <c r="G36" s="24">
+        <v>0</v>
+      </c>
+      <c r="H36" s="24">
+        <v>0</v>
+      </c>
+      <c r="I36" s="24">
+        <v>1012</v>
+      </c>
+      <c r="J36" s="18" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="37" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D37" s="22"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 6/16/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC61948B-20BF-4EB6-A314-D1A5138CF6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0DDD6A-00E7-453E-8B09-55D6FB270282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
   <si>
     <t>Fecha</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>13/6/2025</t>
+  </si>
+  <si>
+    <t>16/6/2025</t>
   </si>
 </sst>
 </file>
@@ -1027,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1729,7 +1732,7 @@
       </c>
     </row>
     <row r="33" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D33" s="21">
+      <c r="D33" s="16">
         <v>45936</v>
       </c>
       <c r="E33" s="3">
@@ -1752,7 +1755,7 @@
       </c>
     </row>
     <row r="34" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D34" s="21">
+      <c r="D34" s="16">
         <v>45967</v>
       </c>
       <c r="E34" s="3">
@@ -1775,7 +1778,7 @@
       </c>
     </row>
     <row r="35" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D35" s="21">
+      <c r="D35" s="16">
         <v>45997</v>
       </c>
       <c r="E35" s="3">
@@ -1821,16 +1824,30 @@
       </c>
     </row>
     <row r="37" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D37" s="22"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="9"/>
+      <c r="D37" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="8">
+        <v>408</v>
+      </c>
+      <c r="F37" s="8">
+        <v>518</v>
+      </c>
+      <c r="G37" s="8">
+        <v>0</v>
+      </c>
+      <c r="H37" s="8">
+        <v>0</v>
+      </c>
+      <c r="I37" s="8">
+        <v>1012</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="38" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D38" s="21"/>
+      <c r="D38" s="16"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -1839,7 +1856,7 @@
       <c r="J38" s="6"/>
     </row>
     <row r="39" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D39" s="21"/>
+      <c r="D39" s="16"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -1848,7 +1865,7 @@
       <c r="J39" s="6"/>
     </row>
     <row r="40" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D40" s="21"/>
+      <c r="D40" s="16"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -1857,7 +1874,7 @@
       <c r="J40" s="6"/>
     </row>
     <row r="41" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D41" s="21"/>
+      <c r="D41" s="16"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
@@ -1866,7 +1883,7 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D42" s="21"/>
+      <c r="D42" s="16"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -1875,7 +1892,7 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D43" s="21"/>
+      <c r="D43" s="16"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -1884,7 +1901,7 @@
       <c r="J43" s="6"/>
     </row>
     <row r="44" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D44" s="22"/>
+      <c r="D44" s="13"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 6/17/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0DDD6A-00E7-453E-8B09-55D6FB270282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90191E82-1527-46F5-BBE2-6CEB7EB90B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
   <si>
     <t>Fecha</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>16/6/2025</t>
+  </si>
+  <si>
+    <t>17/6/2025</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1034,7 @@
   <dimension ref="D2:J45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1847,13 +1850,27 @@
       </c>
     </row>
     <row r="38" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D38" s="16"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="6"/>
+      <c r="D38" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="3">
+        <v>383</v>
+      </c>
+      <c r="F38" s="3">
+        <v>543</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="39" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D39" s="16"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 6/18/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90191E82-1527-46F5-BBE2-6CEB7EB90B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757ED05C-6C8C-4CB6-9BB5-562C57A780CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
   <si>
     <t>Fecha</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>17/6/2025</t>
+  </si>
+  <si>
+    <t>18/6/2025</t>
   </si>
 </sst>
 </file>
@@ -1033,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1873,13 +1876,27 @@
       </c>
     </row>
     <row r="39" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D39" s="16"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="6"/>
+      <c r="D39" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="3">
+        <v>373</v>
+      </c>
+      <c r="F39" s="3">
+        <v>553</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0</v>
+      </c>
+      <c r="I39" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="40" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D40" s="16"/>

</xml_diff>

<commit_message>
Avances Etiquetado Roboflow 6/19/2025
Saludos
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757ED05C-6C8C-4CB6-9BB5-562C57A780CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B20EA6-6142-40C0-9A41-4FA7EE4EAC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
   <si>
     <t>Fecha</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>18/6/2025</t>
+  </si>
+  <si>
+    <t>19/6/2025</t>
+  </si>
+  <si>
+    <t>20/6/2025</t>
+  </si>
+  <si>
+    <t>No he podido adelantar, le dare en fin de semana, disculpa (rafael)</t>
   </si>
 </sst>
 </file>
@@ -1036,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1899,16 +1908,32 @@
       </c>
     </row>
     <row r="40" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D40" s="16"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="6"/>
+      <c r="D40" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="3">
+        <v>373</v>
+      </c>
+      <c r="F40" s="3">
+        <v>553</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
+      <c r="I40" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="41" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D41" s="16"/>
+      <c r="D41" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 6/20/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B20EA6-6142-40C0-9A41-4FA7EE4EAC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3379BF2D-D7DC-44BA-8A5B-086E7D5FB055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
   <si>
     <t>Fecha</t>
   </si>
@@ -1045,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1934,12 +1934,24 @@
       <c r="D41" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="6"/>
+      <c r="E41" s="3">
+        <v>297</v>
+      </c>
+      <c r="F41" s="3">
+        <v>629</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0</v>
+      </c>
+      <c r="I41" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="42" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D42" s="16"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 06/23/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3379BF2D-D7DC-44BA-8A5B-086E7D5FB055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7BACD7-2385-47EA-B7BA-C8A23C5A4B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
   <si>
     <t>Fecha</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>No he podido adelantar, le dare en fin de semana, disculpa (rafael)</t>
+  </si>
+  <si>
+    <t>23/6/2025</t>
   </si>
 </sst>
 </file>
@@ -1045,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1954,13 +1957,27 @@
       </c>
     </row>
     <row r="42" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D42" s="16"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="6"/>
+      <c r="D42" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="3">
+        <v>297</v>
+      </c>
+      <c r="F42" s="3">
+        <v>629</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0</v>
+      </c>
+      <c r="I42" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="43" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D43" s="16"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 6/24/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7BACD7-2385-47EA-B7BA-C8A23C5A4B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D959F110-3991-47D0-8758-3F0CF80B37A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
   <si>
     <t>Fecha</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>23/6/2025</t>
+  </si>
+  <si>
+    <t>24/6/2025</t>
   </si>
 </sst>
 </file>
@@ -1048,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1980,13 +1983,27 @@
       </c>
     </row>
     <row r="43" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D43" s="16"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="6"/>
+      <c r="D43" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43" s="3">
+        <v>297</v>
+      </c>
+      <c r="F43" s="3">
+        <v>629</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="44" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D44" s="13"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 6/25/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D959F110-3991-47D0-8758-3F0CF80B37A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C596484-993A-4D8A-B5EB-4A88A8CA2E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
   <si>
     <t>Fecha</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>24/6/2025</t>
+  </si>
+  <si>
+    <t>25/6/2025</t>
   </si>
 </sst>
 </file>
@@ -1051,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2006,13 +2009,27 @@
       </c>
     </row>
     <row r="44" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D44" s="13"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="9"/>
+      <c r="D44" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44" s="8">
+        <v>297</v>
+      </c>
+      <c r="F44" s="8">
+        <v>629</v>
+      </c>
+      <c r="G44" s="8">
+        <v>0</v>
+      </c>
+      <c r="H44" s="8">
+        <v>0</v>
+      </c>
+      <c r="I44" s="8">
+        <v>1012</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="45" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D45" s="22"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 06/27/2025
Good night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">Etiquetado Roboflow Covenant Drone</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>26/6/2025</t>
+  </si>
+  <si>
+    <t>27/6/2025</t>
   </si>
 </sst>
 </file>
@@ -310,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -356,6 +359,9 @@
     <xf fontId="1" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf fontId="1" fillId="0" borderId="7" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,7 +391,7 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
         <vertical style="none"/>
         <horizontal style="none"/>
       </border>
@@ -415,7 +421,7 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
         <vertical style="none"/>
         <horizontal style="none"/>
       </border>
@@ -445,7 +451,7 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
         <vertical style="none"/>
         <horizontal style="none"/>
       </border>
@@ -475,7 +481,7 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
         <vertical style="none"/>
         <horizontal style="none"/>
       </border>
@@ -505,7 +511,7 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
         <vertical style="none"/>
         <horizontal style="none"/>
       </border>
@@ -535,7 +541,7 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
         <vertical style="none"/>
         <horizontal style="none"/>
       </border>
@@ -563,7 +569,7 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
         <vertical style="none"/>
         <horizontal style="none"/>
       </border>
@@ -582,8 +588,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table1" ref="D4:J45">
-  <autoFilter ref="D4:J45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table1" ref="D4:J46">
+  <autoFilter ref="D4:J46"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Fecha" dataDxfId="0"/>
     <tableColumn id="2" name="Imagenes sin etiquetar" dataDxfId="1"/>
@@ -1098,7 +1104,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A29" zoomScale="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="H29" zoomScale="85" workbookViewId="0">
       <selection activeCell="J45" activeCellId="0" sqref="J45"/>
     </sheetView>
   </sheetViews>
@@ -2095,6 +2101,29 @@
         <v>1012</v>
       </c>
       <c r="J45" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" ht="15">
+      <c r="D46" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" s="17">
+        <v>297</v>
+      </c>
+      <c r="F46" s="17">
+        <v>629</v>
+      </c>
+      <c r="G46" s="17">
+        <v>0</v>
+      </c>
+      <c r="H46" s="17">
+        <v>0</v>
+      </c>
+      <c r="I46" s="17">
+        <v>1012</v>
+      </c>
+      <c r="J46" s="21" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Roboflow Annotation Report 07/01/2025
Good night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC34A1E-E96E-4C58-8C5F-B3EACEE0F5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2762BD62-1EB3-4BD2-BB48-3FCB505A91C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
   <si>
     <t>Fecha</t>
   </si>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2110,13 +2110,27 @@
       </c>
     </row>
     <row r="48" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D48" s="16"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="9"/>
+      <c r="D48" s="16">
+        <v>45664</v>
+      </c>
+      <c r="E48" s="3">
+        <v>192</v>
+      </c>
+      <c r="F48" s="3">
+        <v>734</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0</v>
+      </c>
+      <c r="H48" s="3">
+        <v>0</v>
+      </c>
+      <c r="I48" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J48" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="49" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D49" s="16"/>

</xml_diff>

<commit_message>
Roboflow Image Annotation 7/2/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2762BD62-1EB3-4BD2-BB48-3FCB505A91C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E084C1B-CFFA-4545-9FAA-721812E9AE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
   <si>
     <t>Fecha</t>
   </si>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2133,13 +2133,27 @@
       </c>
     </row>
     <row r="49" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D49" s="16"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="9"/>
+      <c r="D49" s="16">
+        <v>45695</v>
+      </c>
+      <c r="E49" s="3">
+        <v>192</v>
+      </c>
+      <c r="F49" s="3">
+        <v>734</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0</v>
+      </c>
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J49" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="50" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D50" s="16"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/3/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E084C1B-CFFA-4545-9FAA-721812E9AE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04723CE3-5834-4CAB-924B-1D4A10C2DAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
   <si>
     <t>Fecha</t>
   </si>
@@ -1064,7 +1064,7 @@
   <dimension ref="D2:J52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2156,13 +2156,27 @@
       </c>
     </row>
     <row r="50" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D50" s="16"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="9"/>
+      <c r="D50" s="16">
+        <v>45723</v>
+      </c>
+      <c r="E50" s="3">
+        <v>192</v>
+      </c>
+      <c r="F50" s="3">
+        <v>734</v>
+      </c>
+      <c r="G50" s="3">
+        <v>0</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J50" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="51" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D51" s="16"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/4/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04723CE3-5834-4CAB-924B-1D4A10C2DAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115F4F15-AE0E-4425-A6F4-92EC1CC27E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t>Fecha</t>
   </si>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2179,13 +2179,27 @@
       </c>
     </row>
     <row r="51" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D51" s="16"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="9"/>
+      <c r="D51" s="16">
+        <v>45754</v>
+      </c>
+      <c r="E51" s="3">
+        <v>192</v>
+      </c>
+      <c r="F51" s="3">
+        <v>734</v>
+      </c>
+      <c r="G51" s="3">
+        <v>0</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0</v>
+      </c>
+      <c r="I51" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J51" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="52" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D52" s="16"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/7/2025
Se me paso subirlo antes de las 12 mis disculpas
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115F4F15-AE0E-4425-A6F4-92EC1CC27E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10B79A7-9F52-4652-AA2E-24A492C3D711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t>Fecha</t>
   </si>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2202,13 +2202,27 @@
       </c>
     </row>
     <row r="52" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D52" s="16"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="9"/>
+      <c r="D52" s="16">
+        <v>45845</v>
+      </c>
+      <c r="E52" s="3">
+        <v>192</v>
+      </c>
+      <c r="F52" s="3">
+        <v>734</v>
+      </c>
+      <c r="G52" s="3">
+        <v>0</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0</v>
+      </c>
+      <c r="I52" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J52" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/8/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10B79A7-9F52-4652-AA2E-24A492C3D711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD768CB-66D5-4CF1-B71F-9526AE160D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
   <si>
     <t>Fecha</t>
   </si>
@@ -729,8 +729,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J52" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J52" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J53" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J53" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1061,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J52"/>
+  <dimension ref="D2:J53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2221,7 +2221,30 @@
         <v>1012</v>
       </c>
       <c r="J52" s="9" t="s">
-        <v>23</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D53" s="16">
+        <v>45876</v>
+      </c>
+      <c r="E53" s="3">
+        <v>192</v>
+      </c>
+      <c r="F53" s="3">
+        <v>734</v>
+      </c>
+      <c r="G53" s="3">
+        <v>0</v>
+      </c>
+      <c r="H53" s="3">
+        <v>0</v>
+      </c>
+      <c r="I53" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J53" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/9/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD768CB-66D5-4CF1-B71F-9526AE160D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE3281B-E0AE-4D9E-943A-6AC87402C3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
   <si>
     <t>Fecha</t>
   </si>
@@ -729,8 +729,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J53" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J53" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J54" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J54" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1061,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J53"/>
+  <dimension ref="D2:J54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2247,6 +2247,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="54" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D54" s="16">
+        <v>45907</v>
+      </c>
+      <c r="E54" s="3">
+        <v>150</v>
+      </c>
+      <c r="F54" s="3">
+        <v>776</v>
+      </c>
+      <c r="G54" s="3">
+        <v>0</v>
+      </c>
+      <c r="H54" s="3">
+        <v>0</v>
+      </c>
+      <c r="I54" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J54" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/10/2025
Good night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE3281B-E0AE-4D9E-943A-6AC87402C3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4582B69B-6DE2-4A2A-947D-D7CE7233BA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
   <si>
     <t>Fecha</t>
   </si>
@@ -729,8 +729,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J54" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J54" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J56" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J56" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1061,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J54"/>
+  <dimension ref="D2:J56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2270,6 +2270,38 @@
         <v>8</v>
       </c>
     </row>
+    <row r="55" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D55" s="16">
+        <v>45937</v>
+      </c>
+      <c r="E55" s="3">
+        <v>150</v>
+      </c>
+      <c r="F55" s="3">
+        <v>776</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0</v>
+      </c>
+      <c r="H55" s="3">
+        <v>0</v>
+      </c>
+      <c r="I55" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J55" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D56" s="16"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="9"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/11/2025
Good weekend
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4582B69B-6DE2-4A2A-947D-D7CE7233BA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BEE50B-CD9B-4838-A768-1B4CFA6D3696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="44">
   <si>
     <t>Fecha</t>
   </si>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
   <dimension ref="D2:J56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2294,13 +2294,27 @@
       </c>
     </row>
     <row r="56" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D56" s="16"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="9"/>
+      <c r="D56" s="16">
+        <v>45968</v>
+      </c>
+      <c r="E56" s="3">
+        <v>150</v>
+      </c>
+      <c r="F56" s="3">
+        <v>776</v>
+      </c>
+      <c r="G56" s="3">
+        <v>0</v>
+      </c>
+      <c r="H56" s="3">
+        <v>0</v>
+      </c>
+      <c r="I56" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J56" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/14/2025
Good night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BEE50B-CD9B-4838-A768-1B4CFA6D3696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754DC1F3-92D0-46EA-99B8-63AC4BD04A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
   <si>
     <t>Fecha</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>30/6/2025</t>
+  </si>
+  <si>
+    <t>14/7/2025</t>
   </si>
 </sst>
 </file>
@@ -729,8 +732,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J56" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J56" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J57" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J57" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1061,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J56"/>
+  <dimension ref="D2:J57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2316,6 +2319,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="57" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D57" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E57" s="3">
+        <v>150</v>
+      </c>
+      <c r="F57" s="3">
+        <v>776</v>
+      </c>
+      <c r="G57" s="3">
+        <v>0</v>
+      </c>
+      <c r="H57" s="3">
+        <v>0</v>
+      </c>
+      <c r="I57" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/15/2025 (reupload)
Una disculpa, no se porque no se marca el commit en la carpeta, ultimo intento, una disculpa de antemano.
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754DC1F3-92D0-46EA-99B8-63AC4BD04A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981DE9E9-D014-49D7-953E-43EE2434BFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
   <si>
     <t>Fecha</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>14/7/2025</t>
+  </si>
+  <si>
+    <t>14/7/2026</t>
   </si>
 </sst>
 </file>
@@ -732,8 +735,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J57" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J57" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J58" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J58" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1064,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J57"/>
+  <dimension ref="D2:J58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B47" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2342,6 +2345,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="58" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D58" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E58" s="3">
+        <v>75</v>
+      </c>
+      <c r="F58" s="3">
+        <v>851</v>
+      </c>
+      <c r="G58" s="3">
+        <v>0</v>
+      </c>
+      <c r="H58" s="3">
+        <v>0</v>
+      </c>
+      <c r="I58" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J58" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/16/2025
Good day
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981DE9E9-D014-49D7-953E-43EE2434BFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2630AE4-0481-4679-8CE1-6C59F4D687C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
   <si>
     <t>Fecha</t>
   </si>
@@ -173,7 +173,10 @@
     <t>14/7/2025</t>
   </si>
   <si>
-    <t>14/7/2026</t>
+    <t>16/7/2025</t>
+  </si>
+  <si>
+    <t>15/7/2025</t>
   </si>
 </sst>
 </file>
@@ -735,8 +738,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J58" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J58" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J59" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J59" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1067,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J58"/>
+  <dimension ref="D2:J59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B47" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2347,7 +2350,7 @@
     </row>
     <row r="58" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D58" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E58" s="3">
         <v>75</v>
@@ -2365,6 +2368,29 @@
         <v>1012</v>
       </c>
       <c r="J58" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D59" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E59" s="3">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3">
+        <v>924</v>
+      </c>
+      <c r="G59" s="3">
+        <v>0</v>
+      </c>
+      <c r="H59" s="3">
+        <v>0</v>
+      </c>
+      <c r="I59" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J59" s="9" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/17/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2630AE4-0481-4679-8CE1-6C59F4D687C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D5950F-00C8-44A2-B048-ABD926187D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="48">
   <si>
     <t>Fecha</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>15/7/2025</t>
+  </si>
+  <si>
+    <t>17/7/2025</t>
   </si>
 </sst>
 </file>
@@ -738,8 +741,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J59" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J59" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J60" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J60" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1070,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J59"/>
+  <dimension ref="D2:J60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2394,6 +2397,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="60" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D60" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E60" s="3">
+        <v>406</v>
+      </c>
+      <c r="F60" s="3">
+        <v>924</v>
+      </c>
+      <c r="G60" s="3">
+        <v>0</v>
+      </c>
+      <c r="H60" s="3">
+        <v>0</v>
+      </c>
+      <c r="I60" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J60" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/18/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D5950F-00C8-44A2-B048-ABD926187D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C28992-3F2D-4B54-BA33-C6AB0DD9756C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
   <si>
     <t>Fecha</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>17/7/2025</t>
+  </si>
+  <si>
+    <t>18/7/2026</t>
   </si>
 </sst>
 </file>
@@ -741,8 +744,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J60" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J60" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J61" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J61" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1073,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J60"/>
+  <dimension ref="D2:J61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B47" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2420,6 +2423,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="61" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D61" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E61" s="3">
+        <v>406</v>
+      </c>
+      <c r="F61" s="3">
+        <v>924</v>
+      </c>
+      <c r="G61" s="3">
+        <v>0</v>
+      </c>
+      <c r="H61" s="3">
+        <v>0</v>
+      </c>
+      <c r="I61" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J61" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/21/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C28992-3F2D-4B54-BA33-C6AB0DD9756C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2CB60C-338D-4557-9DCB-74CA550EAB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
   <si>
     <t>Fecha</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>18/7/2026</t>
+  </si>
+  <si>
+    <t>21/7/2025</t>
   </si>
 </sst>
 </file>
@@ -744,8 +747,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J61" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J61" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J62" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J62" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1076,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J61"/>
+  <dimension ref="D2:J62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B47" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2446,6 +2449,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="62" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D62" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E62" s="3">
+        <v>406</v>
+      </c>
+      <c r="F62" s="3">
+        <v>924</v>
+      </c>
+      <c r="G62" s="3">
+        <v>0</v>
+      </c>
+      <c r="H62" s="3">
+        <v>0</v>
+      </c>
+      <c r="I62" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J62" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/22/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2CB60C-338D-4557-9DCB-74CA550EAB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DD0230-FE8E-4618-B68C-AAFFDD06E7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="51">
   <si>
     <t>Fecha</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>21/7/2025</t>
+  </si>
+  <si>
+    <t>22/7/2026</t>
   </si>
 </sst>
 </file>
@@ -747,8 +750,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J62" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J62" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J63" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J63" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1079,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J62"/>
+  <dimension ref="D2:J63"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2472,6 +2475,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="63" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D63" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E63" s="3">
+        <v>396</v>
+      </c>
+      <c r="F63" s="3">
+        <v>934</v>
+      </c>
+      <c r="G63" s="3">
+        <v>0</v>
+      </c>
+      <c r="H63" s="3">
+        <v>0</v>
+      </c>
+      <c r="I63" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J63" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/23/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DD0230-FE8E-4618-B68C-AAFFDD06E7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E690B7E7-18FF-4959-A463-AFD2FB81A462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="52">
   <si>
     <t>Fecha</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>22/7/2026</t>
+  </si>
+  <si>
+    <t>23/7/2027</t>
   </si>
 </sst>
 </file>
@@ -750,8 +753,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J63" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J63" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J64" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J64" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1082,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J63"/>
+  <dimension ref="D2:J64"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2498,6 +2501,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="64" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D64" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E64" s="3">
+        <v>380</v>
+      </c>
+      <c r="F64" s="3">
+        <v>950</v>
+      </c>
+      <c r="G64" s="3">
+        <v>0</v>
+      </c>
+      <c r="H64" s="3">
+        <v>0</v>
+      </c>
+      <c r="I64" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J64" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Roboflow annotation report 7/24/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E690B7E7-18FF-4959-A463-AFD2FB81A462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80916757-4B24-4421-A7C6-00D62744C43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
   <si>
     <t>Fecha</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>23/7/2027</t>
+  </si>
+  <si>
+    <t>24/7/2028</t>
   </si>
 </sst>
 </file>
@@ -753,8 +756,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J64" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J64" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J65" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J65" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1085,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J64"/>
+  <dimension ref="D2:J65"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2524,6 +2527,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="65" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D65" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E65" s="3">
+        <v>380</v>
+      </c>
+      <c r="F65" s="3">
+        <v>950</v>
+      </c>
+      <c r="G65" s="3">
+        <v>0</v>
+      </c>
+      <c r="H65" s="3">
+        <v>0</v>
+      </c>
+      <c r="I65" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J65" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/25/2025
Saludos se me olvido subirlo antes de las 12 una disculpa
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80916757-4B24-4421-A7C6-00D62744C43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576DF742-B693-4873-8FEA-5B908969FEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
   <si>
     <t>Fecha</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>24/7/2028</t>
+  </si>
+  <si>
+    <t>25/7/2029</t>
   </si>
 </sst>
 </file>
@@ -756,8 +759,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J65" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J65" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J66" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J66" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1088,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J65"/>
+  <dimension ref="D2:J66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B60" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2550,6 +2553,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="66" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D66" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E66" s="3">
+        <v>380</v>
+      </c>
+      <c r="F66" s="3">
+        <v>950</v>
+      </c>
+      <c r="G66" s="3">
+        <v>0</v>
+      </c>
+      <c r="H66" s="3">
+        <v>0</v>
+      </c>
+      <c r="I66" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J66" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/28/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576DF742-B693-4873-8FEA-5B908969FEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D100A27-8A25-4773-B0AD-EDF46B77BE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="55">
   <si>
     <t>Fecha</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>25/7/2029</t>
+  </si>
+  <si>
+    <t>28/7/2030</t>
   </si>
 </sst>
 </file>
@@ -759,8 +762,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J66" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J66" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J67" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J67" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1091,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J66"/>
+  <dimension ref="D2:J67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B60" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B57" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2576,6 +2579,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="67" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D67" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E67" s="3">
+        <v>380</v>
+      </c>
+      <c r="F67" s="3">
+        <v>950</v>
+      </c>
+      <c r="G67" s="3">
+        <v>0</v>
+      </c>
+      <c r="H67" s="3">
+        <v>0</v>
+      </c>
+      <c r="I67" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J67" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/29/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D100A27-8A25-4773-B0AD-EDF46B77BE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47888B37-03D7-447D-9C54-FC0543BDFFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="56">
   <si>
     <t>Fecha</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>28/7/2030</t>
+  </si>
+  <si>
+    <t>29/7/2031</t>
   </si>
 </sst>
 </file>
@@ -762,8 +765,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J67" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J67" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J68" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J68" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1094,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J67"/>
+  <dimension ref="D2:J68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B57" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2602,6 +2605,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="68" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D68" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E68" s="3">
+        <v>380</v>
+      </c>
+      <c r="F68" s="3">
+        <v>950</v>
+      </c>
+      <c r="G68" s="3">
+        <v>0</v>
+      </c>
+      <c r="H68" s="3">
+        <v>0</v>
+      </c>
+      <c r="I68" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J68" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Roboflow Annotation Report 7/30/2025
Good Night
</commit_message>
<xml_diff>
--- a/datasets/Avances Etiquetado Roboflow.xlsx
+++ b/datasets/Avances Etiquetado Roboflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafar\OneDrive\Escritorio\Nuclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47888B37-03D7-447D-9C54-FC0543BDFFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535D5EF6-B97E-48C6-8AA6-AC1E1C8451D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653B7EE3-2258-482F-9618-3AEEE174FDC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="57">
   <si>
     <t>Fecha</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>29/7/2031</t>
+  </si>
+  <si>
+    <t>30/7/2032</t>
   </si>
 </sst>
 </file>
@@ -765,8 +768,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J68" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="D4:J68" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}" name="Table1" displayName="Table1" ref="D4:J69" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="D4:J69" xr:uid="{4E5E53EA-97EC-41EE-8FA7-CFC9C89A5E4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4C23510A-0932-4F9D-AB34-99275828AC41}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{83CCF2CE-D5FD-4116-8B80-D084E8555FDD}" name="Imagenes sin etiquetar" dataDxfId="5"/>
@@ -1097,9 +1100,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCDBAB-5232-410E-9467-872A79410D6A}">
-  <dimension ref="D2:J68"/>
+  <dimension ref="D2:J69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B59" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
@@ -2628,6 +2631,29 @@
         <v>8</v>
       </c>
     </row>
+    <row r="69" spans="4:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D69" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E69" s="3">
+        <v>329</v>
+      </c>
+      <c r="F69" s="3">
+        <v>1001</v>
+      </c>
+      <c r="G69" s="3">
+        <v>0</v>
+      </c>
+      <c r="H69" s="3">
+        <v>0</v>
+      </c>
+      <c r="I69" s="3">
+        <v>1012</v>
+      </c>
+      <c r="J69" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>